<commit_message>
Mostrar rango cuando le doy al nivel de dificultad
</commit_message>
<xml_diff>
--- a/Proyecto/DatosInformeCalidad.xlsx
+++ b/Proyecto/DatosInformeCalidad.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alba\Escritorio\1.UEM\2021-2022\1 cuatrimestre\Proyecto\Proyecto matlab\TrackMotion\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DANIELBAQUEROZAZO\Documents\MATLAB\TrackMotion\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD34DA29-56C6-4B87-8242-3E2E765BBB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B1A748-5841-4006-8718-8CA51EDCFA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="10188" windowHeight="8964" xr2:uid="{A06EA087-EB8B-44B9-B597-380F78CDFBAC}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{A06EA087-EB8B-44B9-B597-380F78CDFBAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -436,12 +434,12 @@
       <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -478,22 +476,22 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>71.128871128871126</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>73.2</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>22.886886201271473</v>
+        <v>22.810807399706093</v>
       </c>
       <c r="G2">
-        <v>62.886886201271473</v>
+        <v>62.810807399706093</v>
       </c>
       <c r="H2">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -504,22 +502,22 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>71.128871128871126</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>74.2</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>27.34275463129169</v>
+        <v>28.19861889156364</v>
       </c>
       <c r="G3">
-        <v>37.34275463129169</v>
+        <v>38.19861889156364</v>
       </c>
       <c r="H3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -530,22 +528,22 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>71.128871128871126</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>56.8</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>57.356900041311306</v>
+        <v>56.378670739293071</v>
       </c>
       <c r="G4">
-        <v>122.55401165399701</v>
+        <v>122.28134913072228</v>
       </c>
       <c r="H4">
-        <v>65.197111612685703</v>
+        <v>65.902678391429205</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -556,22 +554,22 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>71.128871128871126</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>77.099999999999994</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>39.423343765593444</v>
+        <v>43.355339105518681</v>
       </c>
       <c r="G5">
-        <v>57.522638242998568</v>
+        <v>57.986070536640781</v>
       </c>
       <c r="H5">
-        <v>18.099294477405127</v>
+        <v>14.630731431122097</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -582,22 +580,22 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>71.128871128871126</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>71.7</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>15.604003131001303</v>
+        <v>16.43556202943499</v>
       </c>
       <c r="G6">
-        <v>20.604003131001303</v>
+        <v>21.43556202943499</v>
       </c>
       <c r="H6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -608,19 +606,19 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>71.128871128871126</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>74.2</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>7.8418971196848517</v>
+        <v>6.2731813929354026</v>
       </c>
       <c r="G7">
-        <v>31.38272493716569</v>
+        <v>29.851647229533484</v>
       </c>
       <c r="H7">
-        <v>23.540827817480839</v>
+        <v>23.578465836598081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>